<commit_message>
- push version - adds support of the Lebrew RoastSee NEXT - adds possibility to overwrite the event button value on alarm action `Event Button`
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/alarms.xlsx
+++ b/doc/help_dialogs/Input_files/alarms.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Alarms" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Options" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Actions" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Alarms" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Options" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Actions" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -217,10 +217,28 @@
     <t xml:space="preserve">Event Button</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;button number&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triggers the button, the button number comes from the Events Buttons configuration</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;button number&gt;[&gt;&lt;value&gt;],..,&lt;button number&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[&gt;&lt;value&gt;]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">triggers the button optional overwriting the button value with &lt;value&gt; (eg. ‘1&gt;10,2,3&gt;100’); the button number comes from the Events Buttons configuration</t>
   </si>
   <si>
     <t xml:space="preserve">Slider &lt;1&gt;</t>
@@ -345,7 +363,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -373,6 +391,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -417,20 +441,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -446,132 +474,238 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="50.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="87.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -581,7 +715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -593,130 +727,130 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="71.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -726,239 +860,239 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="66.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="66.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+    <row r="24" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
- adds Phidget drivers explicitly to mac/linux builds - translation updates
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/alarms.xlsx
+++ b/doc/help_dialogs/Input_files/alarms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Alarms" sheetId="1" state="visible" r:id="rId3"/>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">The action to be triggered if all conditions are fulfilled.</t>
   </si>
   <si>
-    <t xml:space="preserve">Commands for alarms with an action go here.  Anything after a '#' character is considered a comment and is ignored when processing the alarm.  </t>
+    <t xml:space="preserve">Commands for alarms with an action go here.  Anything after a '#' character is considered a comment and is ignored when processing the alarm.</t>
   </si>
   <si>
     <t xml:space="preserve">ALARM CONFIGURATION OPTIONS</t>
@@ -217,25 +217,7 @@
     <t xml:space="preserve">Event Button</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;button number&gt;[&gt;&lt;value&gt;],..,&lt;button number&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[&gt;&lt;value&gt;]</t>
-    </r>
+    <t xml:space="preserve">&lt;button number&gt;[&gt;&lt;value&gt;],..,&lt;button number&gt;[&gt;&lt;value&gt;]</t>
   </si>
   <si>
     <t xml:space="preserve">triggers the button optional overwriting the button value with &lt;value&gt; (eg. ‘1&gt;10,2,3&gt;100’); the button number comes from the Events Buttons configuration</t>
@@ -363,7 +345,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -391,12 +373,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -587,7 +563,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -866,7 +842,7 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>